<commit_message>
hot fix. Wrong sample data attached.
</commit_message>
<xml_diff>
--- a/public/sample-exported-data.xlsx
+++ b/public/sample-exported-data.xlsx
@@ -12,9 +12,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
-  <si>
-    <t>sex</t>
-  </si>
   <si>
     <t>Date of Birth</t>
   </si>
@@ -35,6 +32,9 @@
   </si>
   <si>
     <t>Nationality</t>
+  </si>
+  <si>
+    <t>Sex</t>
   </si>
   <si>
     <t>NRIC Number</t>
@@ -64,18 +64,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -88,16 +82,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -107,17 +101,14 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -137,7 +128,6 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -289,9 +279,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
+                <a:alpha val="38000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -371,7 +361,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -398,10 +388,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -648,9 +638,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="35000"/>
+              <a:alpha val="38000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -928,7 +918,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -955,10 +945,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1203,7 +1193,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1242,105 +1232,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" ht="15.35" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" ht="15.35" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" ht="15.35" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" ht="15.35" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" ht="15.35" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" ht="15.35" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" ht="15.35" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" ht="15.35" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" ht="15.35" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>